<commit_message>
AI relevance check file make
</commit_message>
<xml_diff>
--- a/research_pp_qa/new_not_in_old_df.xlsx
+++ b/research_pp_qa/new_not_in_old_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Documents\Evident-Work\research_pp_qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD049D1-C0C7-4DD8-9463-ABF2D03F0429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64A8A1B-56B2-4748-9B1E-209BB15567B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="255">
   <si>
     <t>paper_url</t>
   </si>
@@ -1164,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1404,7 +1404,7 @@
         <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="156.75" x14ac:dyDescent="0.45">
@@ -1490,6 +1490,9 @@
       <c r="H11" t="s">
         <v>22</v>
       </c>
+      <c r="I11" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="242.25" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
@@ -1516,6 +1519,9 @@
       <c r="H12" t="s">
         <v>22</v>
       </c>
+      <c r="I12" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="171" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
@@ -1541,6 +1547,9 @@
       </c>
       <c r="H13" t="s">
         <v>42</v>
+      </c>
+      <c r="I13" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="156.75" x14ac:dyDescent="0.45">
@@ -1568,6 +1577,9 @@
       <c r="H14" t="s">
         <v>64</v>
       </c>
+      <c r="I14" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="299.25" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
@@ -1594,6 +1606,9 @@
       <c r="H15" t="s">
         <v>42</v>
       </c>
+      <c r="I15" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
@@ -1620,8 +1635,11 @@
       <c r="H16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="I16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1643,8 +1661,11 @@
       <c r="H17" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="I17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1669,8 +1690,11 @@
       <c r="H18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="I18" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1695,8 +1719,11 @@
       <c r="H19" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="I19" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1718,8 +1745,11 @@
       <c r="H20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="I20" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1744,8 +1774,11 @@
       <c r="H21" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="I21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1770,8 +1803,11 @@
       <c r="H22" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="I22" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1797,7 +1833,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="171" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" ht="171" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1823,7 +1859,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1846,7 +1882,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1872,7 +1908,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="285" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" ht="285" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1898,7 +1934,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1924,7 +1960,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1950,7 +1986,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1976,7 +2012,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" ht="199.5" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2002,7 +2038,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>30</v>
       </c>

</xml_diff>